<commit_message>
Update CrashAndBack in Durable
</commit_message>
<xml_diff>
--- a/ExperimentRecord.xlsx
+++ b/ExperimentRecord.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dh/Projects/mongodb-tunable-consistency-tla/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0E6D29-EC2C-4446-83C6-9C9AA3A86BA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CD2FEC-1101-DA44-92CD-04C1E46D66BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="500" windowWidth="28240" windowHeight="16100" activeTab="1" xr2:uid="{493B68AF-54D3-6E4F-9EF2-7D5F13399502}"/>
+    <workbookView xWindow="560" yWindow="500" windowWidth="28240" windowHeight="16040" activeTab="2" xr2:uid="{493B68AF-54D3-6E4F-9EF2-7D5F13399502}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic_problemoverflow" sheetId="1" r:id="rId1"/>
     <sheet name="Basic" sheetId="2" r:id="rId2"/>
+    <sheet name="Durable" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -638,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37FAD5C9-7D39-9D44-B652-8D74FBCAA18D}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -884,6 +885,21 @@
       <c r="C10" s="2">
         <v>5</v>
       </c>
+      <c r="D10" s="2">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2">
+        <v>309501013</v>
+      </c>
+      <c r="F10" s="2">
+        <v>100000096</v>
+      </c>
+      <c r="G10" s="2">
+        <v>80098733</v>
+      </c>
+      <c r="H10" s="3">
+        <v>4.8888888888888891E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="2">
@@ -895,6 +911,21 @@
       <c r="C11" s="2">
         <v>2</v>
       </c>
+      <c r="D11" s="2">
+        <v>14</v>
+      </c>
+      <c r="E11" s="2">
+        <v>330785622</v>
+      </c>
+      <c r="F11" s="2">
+        <v>100000030</v>
+      </c>
+      <c r="G11" s="2">
+        <v>78511175</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.20518518518518516</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="2">
@@ -906,6 +937,21 @@
       <c r="C12" s="2">
         <v>3</v>
       </c>
+      <c r="D12" s="2">
+        <v>14</v>
+      </c>
+      <c r="E12" s="2">
+        <v>335953465</v>
+      </c>
+      <c r="F12" s="2">
+        <v>100000040</v>
+      </c>
+      <c r="G12" s="2">
+        <v>79041186</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.21305555555555555</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="2">
@@ -917,6 +963,21 @@
       <c r="C13" s="2">
         <v>4</v>
       </c>
+      <c r="D13" s="2">
+        <v>13</v>
+      </c>
+      <c r="E13" s="2">
+        <v>341161320</v>
+      </c>
+      <c r="F13" s="2">
+        <v>100000068</v>
+      </c>
+      <c r="G13" s="2">
+        <v>79339459</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.24410879629629631</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="2">
@@ -928,6 +989,21 @@
       <c r="C14" s="2">
         <v>5</v>
       </c>
+      <c r="D14" s="2">
+        <v>13</v>
+      </c>
+      <c r="E14" s="2">
+        <v>341846423</v>
+      </c>
+      <c r="F14" s="2">
+        <v>100000073</v>
+      </c>
+      <c r="G14" s="2">
+        <v>79774012</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0.28657407407407409</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="2">
@@ -939,6 +1015,21 @@
       <c r="C15" s="2">
         <v>2</v>
       </c>
+      <c r="D15" s="2">
+        <v>13</v>
+      </c>
+      <c r="E15" s="2">
+        <v>386115817</v>
+      </c>
+      <c r="F15" s="2">
+        <v>100000045</v>
+      </c>
+      <c r="G15" s="2">
+        <v>80671850</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0.52913194444444445</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="2">
@@ -950,8 +1041,23 @@
       <c r="C16" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" s="2">
+        <v>13</v>
+      </c>
+      <c r="E16" s="2">
+        <v>367708286</v>
+      </c>
+      <c r="F16" s="2">
+        <v>100000121</v>
+      </c>
+      <c r="G16" s="2">
+        <v>82091596</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0.57899305555555558</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="2">
         <v>5</v>
       </c>
@@ -961,8 +1067,23 @@
       <c r="C17" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" s="2">
+        <v>11</v>
+      </c>
+      <c r="E17" s="2">
+        <v>395682063</v>
+      </c>
+      <c r="F17" s="2">
+        <v>100000075</v>
+      </c>
+      <c r="G17" s="2">
+        <v>81634279</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0.74784722222222222</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="2">
         <v>5</v>
       </c>
@@ -971,6 +1092,21 @@
       </c>
       <c r="C18" s="2">
         <v>5</v>
+      </c>
+      <c r="D18" s="2">
+        <v>12</v>
+      </c>
+      <c r="E18" s="2">
+        <v>401141644</v>
+      </c>
+      <c r="F18" s="2">
+        <v>100000047</v>
+      </c>
+      <c r="G18" s="2">
+        <v>82182689</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0.7575115740740741</v>
       </c>
     </row>
   </sheetData>
@@ -985,4 +1121,19 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56A55845-5592-2947-A858-45AACE99DB57}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update: change snapshot into a inherent action when local store changes
</commit_message>
<xml_diff>
--- a/ExperimentRecord.xlsx
+++ b/ExperimentRecord.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dh/Projects/mongodb-tunable-consistency-tla/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CD2FEC-1101-DA44-92CD-04C1E46D66BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8744AA59-DBFF-0C42-AC63-774E383380E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="500" windowWidth="28240" windowHeight="16040" activeTab="2" xr2:uid="{493B68AF-54D3-6E4F-9EF2-7D5F13399502}"/>
+    <workbookView xWindow="540" yWindow="760" windowWidth="28240" windowHeight="16040" activeTab="2" xr2:uid="{493B68AF-54D3-6E4F-9EF2-7D5F13399502}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic_problemoverflow" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>TLC模型</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -63,13 +63,40 @@
   <si>
     <t>Queue Size</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TLC模型</t>
+  </si>
+  <si>
+    <t>状态图直径</t>
+  </si>
+  <si>
+    <t>状态数</t>
+  </si>
+  <si>
+    <t>不同状态数</t>
+  </si>
+  <si>
+    <t>Queue Size</t>
+  </si>
+  <si>
+    <t>检验时间</t>
+  </si>
+  <si>
+    <t>Server Num</t>
+  </si>
+  <si>
+    <t>Client Num</t>
+  </si>
+  <si>
+    <t>Key Num</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -82,6 +109,13 @@
       <sz val="9"/>
       <name val="等线"/>
       <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -108,7 +142,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -121,7 +155,16 @@
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -454,24 +497,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="E1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -485,11 +528,11 @@
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1">
@@ -640,7 +683,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -656,24 +699,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="E1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -687,11 +730,11 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2">
@@ -1125,14 +1168,427 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56A55845-5592-2947-A858-45AACE99DB57}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="4">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>15</v>
+      </c>
+      <c r="E3" s="4">
+        <v>351846374</v>
+      </c>
+      <c r="F3" s="4">
+        <v>100000027</v>
+      </c>
+      <c r="G3" s="4">
+        <v>68427817</v>
+      </c>
+      <c r="H3" s="5">
+        <v>4.297453703703704E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4">
+        <v>349869869</v>
+      </c>
+      <c r="F4" s="4">
+        <v>100000016</v>
+      </c>
+      <c r="G4" s="4">
+        <v>69236467</v>
+      </c>
+      <c r="H4" s="5">
+        <v>4.4016203703703703E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4">
+        <v>4</v>
+      </c>
+      <c r="D5" s="4">
+        <v>14</v>
+      </c>
+      <c r="E5" s="4">
+        <v>347023882</v>
+      </c>
+      <c r="F5" s="4">
+        <v>100000029</v>
+      </c>
+      <c r="G5" s="4">
+        <v>69791592</v>
+      </c>
+      <c r="H5" s="5">
+        <v>4.2465277777777775E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="4">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4">
+        <v>2</v>
+      </c>
+      <c r="C6" s="4">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4">
+        <v>14</v>
+      </c>
+      <c r="E6" s="4">
+        <v>346545192</v>
+      </c>
+      <c r="F6" s="4">
+        <v>100000012</v>
+      </c>
+      <c r="G6" s="4">
+        <v>70234362</v>
+      </c>
+      <c r="H6" s="5">
+        <v>4.2928240740740746E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="4">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4">
+        <v>3</v>
+      </c>
+      <c r="C7" s="4">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4">
+        <v>13</v>
+      </c>
+      <c r="E7" s="4">
+        <v>364402539</v>
+      </c>
+      <c r="F7" s="4">
+        <v>100000041</v>
+      </c>
+      <c r="G7" s="4">
+        <v>73860653</v>
+      </c>
+      <c r="H7" s="5">
+        <v>6.5995370370370371E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="4">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4">
+        <v>3</v>
+      </c>
+      <c r="C8" s="4">
+        <v>3</v>
+      </c>
+      <c r="D8" s="4">
+        <v>13</v>
+      </c>
+      <c r="E8" s="4">
+        <v>373571942</v>
+      </c>
+      <c r="F8" s="4">
+        <v>100000035</v>
+      </c>
+      <c r="G8" s="4">
+        <v>74975922</v>
+      </c>
+      <c r="H8" s="5">
+        <v>7.1319444444444449E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="4">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4">
+        <v>3</v>
+      </c>
+      <c r="C9" s="4">
+        <v>4</v>
+      </c>
+      <c r="D9" s="4">
+        <v>13</v>
+      </c>
+      <c r="E9" s="4">
+        <v>381596426</v>
+      </c>
+      <c r="F9" s="4">
+        <v>100000054</v>
+      </c>
+      <c r="G9" s="4">
+        <v>75905896</v>
+      </c>
+      <c r="H9" s="5">
+        <v>7.3124999999999996E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="4">
+        <v>3</v>
+      </c>
+      <c r="B10" s="4">
+        <v>3</v>
+      </c>
+      <c r="C10" s="4">
+        <v>5</v>
+      </c>
+      <c r="D10" s="4">
+        <v>12</v>
+      </c>
+      <c r="E10" s="4">
+        <v>379711195</v>
+      </c>
+      <c r="F10" s="4">
+        <v>100000017</v>
+      </c>
+      <c r="G10" s="4">
+        <v>76533973</v>
+      </c>
+      <c r="H10" s="5">
+        <v>7.8032407407407411E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="4">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4">
+        <v>2</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2</v>
+      </c>
+      <c r="D11" s="4">
+        <v>13</v>
+      </c>
+      <c r="E11" s="4">
+        <v>377009534</v>
+      </c>
+      <c r="F11" s="4">
+        <v>100000037</v>
+      </c>
+      <c r="G11" s="4">
+        <v>79540261</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0.32546296296296295</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="4">
+        <v>5</v>
+      </c>
+      <c r="B12" s="4">
+        <v>2</v>
+      </c>
+      <c r="C12" s="4">
+        <v>3</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="4">
+        <v>5</v>
+      </c>
+      <c r="B13" s="4">
+        <v>2</v>
+      </c>
+      <c r="C13" s="4">
+        <v>4</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="4">
+        <v>5</v>
+      </c>
+      <c r="B14" s="4">
+        <v>2</v>
+      </c>
+      <c r="C14" s="4">
+        <v>5</v>
+      </c>
+      <c r="D14" s="4">
+        <v>13</v>
+      </c>
+      <c r="E14" s="4">
+        <v>414728822</v>
+      </c>
+      <c r="F14" s="4">
+        <v>100000042</v>
+      </c>
+      <c r="G14" s="4">
+        <v>79483016</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0.41244212962962962</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="4">
+        <v>5</v>
+      </c>
+      <c r="B15" s="4">
+        <v>3</v>
+      </c>
+      <c r="C15" s="4">
+        <v>2</v>
+      </c>
+      <c r="D15" s="4">
+        <v>13</v>
+      </c>
+      <c r="E15" s="4">
+        <v>463905335</v>
+      </c>
+      <c r="F15" s="4">
+        <v>100000022</v>
+      </c>
+      <c r="G15" s="4">
+        <v>80998636</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0.89020833333333327</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="4">
+        <v>5</v>
+      </c>
+      <c r="B16" s="4">
+        <v>3</v>
+      </c>
+      <c r="C16" s="4">
+        <v>3</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="4">
+        <v>5</v>
+      </c>
+      <c r="B17" s="4">
+        <v>3</v>
+      </c>
+      <c r="C17" s="4">
+        <v>4</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="4">
+        <v>5</v>
+      </c>
+      <c r="B18" s="4">
+        <v>3</v>
+      </c>
+      <c r="C18" s="4">
+        <v>5</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update CMvSpec: Only consider definition in (vis,ar,V) now
</commit_message>
<xml_diff>
--- a/ExperimentRecord.xlsx
+++ b/ExperimentRecord.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dh/Projects/mongodb-tunable-consistency-tla/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8744AA59-DBFF-0C42-AC63-774E383380E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B207AF-D38A-944C-9038-C685F3188BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="760" windowWidth="28240" windowHeight="16040" activeTab="2" xr2:uid="{493B68AF-54D3-6E4F-9EF2-7D5F13399502}"/>
+    <workbookView xWindow="540" yWindow="760" windowWidth="28240" windowHeight="16040" activeTab="4" xr2:uid="{493B68AF-54D3-6E4F-9EF2-7D5F13399502}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic_problemoverflow" sheetId="1" r:id="rId1"/>
     <sheet name="Basic" sheetId="2" r:id="rId2"/>
     <sheet name="Durable" sheetId="3" r:id="rId3"/>
+    <sheet name="Durable2" sheetId="4" r:id="rId4"/>
+    <sheet name="Recoverable" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="18">
   <si>
     <t>TLC模型</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -96,7 +98,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -116,6 +118,22 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -142,7 +160,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -165,6 +183,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -683,7 +716,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1170,8 +1203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56A55845-5592-2947-A858-45AACE99DB57}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1592,4 +1625,780 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D669FEF8-2D6A-7B4F-B00F-588A1C104E82}">
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="8">
+        <v>3</v>
+      </c>
+      <c r="B3" s="8">
+        <v>2</v>
+      </c>
+      <c r="C3" s="8">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8">
+        <v>15</v>
+      </c>
+      <c r="E3" s="8">
+        <v>351846374</v>
+      </c>
+      <c r="F3" s="8">
+        <v>100000027</v>
+      </c>
+      <c r="G3" s="8">
+        <v>68427817</v>
+      </c>
+      <c r="H3" s="9">
+        <v>4.297453703703704E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8">
+        <v>2</v>
+      </c>
+      <c r="C4" s="8">
+        <v>3</v>
+      </c>
+      <c r="D4" s="8">
+        <v>15</v>
+      </c>
+      <c r="E4" s="8">
+        <v>349869869</v>
+      </c>
+      <c r="F4" s="8">
+        <v>100000016</v>
+      </c>
+      <c r="G4" s="8">
+        <v>69236467</v>
+      </c>
+      <c r="H4" s="9">
+        <v>4.4016203703703703E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="8">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8">
+        <v>2</v>
+      </c>
+      <c r="C5" s="8">
+        <v>4</v>
+      </c>
+      <c r="D5" s="8">
+        <v>14</v>
+      </c>
+      <c r="E5" s="8">
+        <v>347023882</v>
+      </c>
+      <c r="F5" s="8">
+        <v>100000029</v>
+      </c>
+      <c r="G5" s="8">
+        <v>69791592</v>
+      </c>
+      <c r="H5" s="9">
+        <v>4.2465277777777775E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="8">
+        <v>3</v>
+      </c>
+      <c r="B6" s="8">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8">
+        <v>5</v>
+      </c>
+      <c r="D6" s="8">
+        <v>14</v>
+      </c>
+      <c r="E6" s="8">
+        <v>346545192</v>
+      </c>
+      <c r="F6" s="8">
+        <v>100000012</v>
+      </c>
+      <c r="G6" s="8">
+        <v>70234362</v>
+      </c>
+      <c r="H6" s="9">
+        <v>4.2928240740740746E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="8">
+        <v>3</v>
+      </c>
+      <c r="B7" s="8">
+        <v>3</v>
+      </c>
+      <c r="C7" s="8">
+        <v>2</v>
+      </c>
+      <c r="D7" s="8">
+        <v>13</v>
+      </c>
+      <c r="E7" s="8">
+        <v>364402539</v>
+      </c>
+      <c r="F7" s="8">
+        <v>100000041</v>
+      </c>
+      <c r="G7" s="8">
+        <v>73860653</v>
+      </c>
+      <c r="H7" s="9">
+        <v>6.5995370370370371E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="8">
+        <v>3</v>
+      </c>
+      <c r="B8" s="8">
+        <v>3</v>
+      </c>
+      <c r="C8" s="8">
+        <v>3</v>
+      </c>
+      <c r="D8" s="8">
+        <v>13</v>
+      </c>
+      <c r="E8" s="8">
+        <v>373571942</v>
+      </c>
+      <c r="F8" s="8">
+        <v>100000035</v>
+      </c>
+      <c r="G8" s="8">
+        <v>74975922</v>
+      </c>
+      <c r="H8" s="9">
+        <v>7.1319444444444449E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="8">
+        <v>3</v>
+      </c>
+      <c r="B9" s="8">
+        <v>3</v>
+      </c>
+      <c r="C9" s="8">
+        <v>4</v>
+      </c>
+      <c r="D9" s="8">
+        <v>13</v>
+      </c>
+      <c r="E9" s="8">
+        <v>381596426</v>
+      </c>
+      <c r="F9" s="8">
+        <v>100000054</v>
+      </c>
+      <c r="G9" s="8">
+        <v>75905896</v>
+      </c>
+      <c r="H9" s="9">
+        <v>7.3124999999999996E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="8">
+        <v>3</v>
+      </c>
+      <c r="B10" s="8">
+        <v>3</v>
+      </c>
+      <c r="C10" s="8">
+        <v>5</v>
+      </c>
+      <c r="D10" s="8">
+        <v>13</v>
+      </c>
+      <c r="E10" s="11">
+        <v>327918897</v>
+      </c>
+      <c r="F10" s="11">
+        <v>100000033</v>
+      </c>
+      <c r="G10" s="11">
+        <v>72522258</v>
+      </c>
+      <c r="H10" s="12">
+        <v>7.9432870370370376E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="8">
+        <v>5</v>
+      </c>
+      <c r="B11" s="8">
+        <v>2</v>
+      </c>
+      <c r="C11" s="8">
+        <v>2</v>
+      </c>
+      <c r="D11" s="8">
+        <v>15</v>
+      </c>
+      <c r="E11" s="11">
+        <v>294507237</v>
+      </c>
+      <c r="F11" s="11">
+        <v>100000050</v>
+      </c>
+      <c r="G11" s="11">
+        <v>76383090</v>
+      </c>
+      <c r="H11" s="12">
+        <v>0.26369212962962962</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="8">
+        <v>5</v>
+      </c>
+      <c r="B12" s="8">
+        <v>2</v>
+      </c>
+      <c r="C12" s="8">
+        <v>3</v>
+      </c>
+      <c r="D12" s="8">
+        <v>14</v>
+      </c>
+      <c r="E12" s="11">
+        <v>307431446</v>
+      </c>
+      <c r="F12" s="11">
+        <v>100000037</v>
+      </c>
+      <c r="G12" s="11">
+        <v>76311354</v>
+      </c>
+      <c r="H12" s="12">
+        <v>0.31482638888888886</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="8">
+        <v>5</v>
+      </c>
+      <c r="B13" s="8">
+        <v>2</v>
+      </c>
+      <c r="C13" s="8">
+        <v>4</v>
+      </c>
+      <c r="D13" s="8">
+        <v>13</v>
+      </c>
+      <c r="E13" s="11">
+        <v>300430635</v>
+      </c>
+      <c r="F13" s="11">
+        <v>100000020</v>
+      </c>
+      <c r="G13" s="11">
+        <v>76718798</v>
+      </c>
+      <c r="H13" s="12">
+        <v>0.31440972222222224</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="8">
+        <v>5</v>
+      </c>
+      <c r="B14" s="8">
+        <v>2</v>
+      </c>
+      <c r="C14" s="8">
+        <v>5</v>
+      </c>
+      <c r="D14" s="8">
+        <v>14</v>
+      </c>
+      <c r="E14" s="11">
+        <v>310525002</v>
+      </c>
+      <c r="F14" s="11">
+        <v>100000015</v>
+      </c>
+      <c r="G14" s="11">
+        <v>76639328</v>
+      </c>
+      <c r="H14" s="12">
+        <v>0.34306712962962965</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="8">
+        <v>5</v>
+      </c>
+      <c r="B15" s="8">
+        <v>3</v>
+      </c>
+      <c r="C15" s="8">
+        <v>2</v>
+      </c>
+      <c r="D15" s="8">
+        <v>13</v>
+      </c>
+      <c r="E15" s="8">
+        <v>463905335</v>
+      </c>
+      <c r="F15" s="8">
+        <v>100000022</v>
+      </c>
+      <c r="G15" s="8">
+        <v>80998636</v>
+      </c>
+      <c r="H15" s="9">
+        <v>0.89020833333333327</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="8">
+        <v>5</v>
+      </c>
+      <c r="B16" s="8">
+        <v>3</v>
+      </c>
+      <c r="C16" s="8">
+        <v>3</v>
+      </c>
+      <c r="D16" s="8">
+        <v>13</v>
+      </c>
+      <c r="E16" s="11">
+        <v>386554906</v>
+      </c>
+      <c r="F16" s="11">
+        <v>100000013</v>
+      </c>
+      <c r="G16" s="11">
+        <v>78922503</v>
+      </c>
+      <c r="H16" s="12">
+        <v>0.94987268518518519</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="8">
+        <v>5</v>
+      </c>
+      <c r="B17" s="8">
+        <v>3</v>
+      </c>
+      <c r="C17" s="8">
+        <v>4</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="8">
+        <v>5</v>
+      </c>
+      <c r="B18" s="8">
+        <v>3</v>
+      </c>
+      <c r="C18" s="8">
+        <v>5</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B6E2F82-D946-0145-A470-82D88D964591}">
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="8">
+        <v>3</v>
+      </c>
+      <c r="B3" s="8">
+        <v>2</v>
+      </c>
+      <c r="C3" s="8">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8">
+        <v>2</v>
+      </c>
+      <c r="C4" s="8">
+        <v>3</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="8">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8">
+        <v>2</v>
+      </c>
+      <c r="C5" s="8">
+        <v>4</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="8">
+        <v>3</v>
+      </c>
+      <c r="B6" s="8">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8">
+        <v>5</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="8">
+        <v>3</v>
+      </c>
+      <c r="B7" s="8">
+        <v>3</v>
+      </c>
+      <c r="C7" s="8">
+        <v>2</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="8">
+        <v>3</v>
+      </c>
+      <c r="B8" s="8">
+        <v>3</v>
+      </c>
+      <c r="C8" s="8">
+        <v>3</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="8">
+        <v>3</v>
+      </c>
+      <c r="B9" s="8">
+        <v>3</v>
+      </c>
+      <c r="C9" s="8">
+        <v>4</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="8">
+        <v>3</v>
+      </c>
+      <c r="B10" s="8">
+        <v>3</v>
+      </c>
+      <c r="C10" s="8">
+        <v>5</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="12"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="8">
+        <v>5</v>
+      </c>
+      <c r="B11" s="8">
+        <v>2</v>
+      </c>
+      <c r="C11" s="8">
+        <v>2</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="12"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="8">
+        <v>5</v>
+      </c>
+      <c r="B12" s="8">
+        <v>2</v>
+      </c>
+      <c r="C12" s="8">
+        <v>3</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="12"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="8">
+        <v>5</v>
+      </c>
+      <c r="B13" s="8">
+        <v>2</v>
+      </c>
+      <c r="C13" s="8">
+        <v>4</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="12"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="8">
+        <v>5</v>
+      </c>
+      <c r="B14" s="8">
+        <v>2</v>
+      </c>
+      <c r="C14" s="8">
+        <v>5</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="12"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="8">
+        <v>5</v>
+      </c>
+      <c r="B15" s="8">
+        <v>3</v>
+      </c>
+      <c r="C15" s="8">
+        <v>2</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="9"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="8">
+        <v>5</v>
+      </c>
+      <c r="B16" s="8">
+        <v>3</v>
+      </c>
+      <c r="C16" s="8">
+        <v>3</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="12"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="8">
+        <v>5</v>
+      </c>
+      <c r="B17" s="8">
+        <v>3</v>
+      </c>
+      <c r="C17" s="8">
+        <v>4</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="8">
+        <v>5</v>
+      </c>
+      <c r="B18" s="8">
+        <v>3</v>
+      </c>
+      <c r="C18" s="8">
+        <v>5</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Checkpoint before modification: omit the delay between server and client
</commit_message>
<xml_diff>
--- a/ExperimentRecord.xlsx
+++ b/ExperimentRecord.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dh/Projects/mongodb-tunable-consistency-tla/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B207AF-D38A-944C-9038-C685F3188BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EC7D30-3B8B-5D41-8689-83517A909391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="760" windowWidth="28240" windowHeight="16040" activeTab="4" xr2:uid="{493B68AF-54D3-6E4F-9EF2-7D5F13399502}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" activeTab="3" xr2:uid="{493B68AF-54D3-6E4F-9EF2-7D5F13399502}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic_problemoverflow" sheetId="1" r:id="rId1"/>
@@ -98,7 +98,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -137,6 +137,22 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -160,7 +176,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -198,6 +214,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="21" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -716,7 +744,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1204,7 +1232,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1491,11 +1519,21 @@
       <c r="C12" s="4">
         <v>3</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="D12" s="13">
+        <v>14</v>
+      </c>
+      <c r="E12" s="13">
+        <v>307768923</v>
+      </c>
+      <c r="F12" s="13">
+        <v>100000035</v>
+      </c>
+      <c r="G12" s="13">
+        <v>76287928</v>
+      </c>
+      <c r="H12" s="14">
+        <v>0.29973379629629632</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="4">
@@ -1631,8 +1669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D669FEF8-2D6A-7B4F-B00F-588A1C104E82}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2089,8 +2127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B6E2F82-D946-0145-A470-82D88D964591}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2143,11 +2181,21 @@
       <c r="C3" s="8">
         <v>2</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="9"/>
+      <c r="D3" s="8">
+        <v>13</v>
+      </c>
+      <c r="E3" s="8">
+        <v>262093595</v>
+      </c>
+      <c r="F3" s="8">
+        <v>100000032</v>
+      </c>
+      <c r="G3" s="8">
+        <v>83587462</v>
+      </c>
+      <c r="H3" s="9">
+        <v>4.0300925925925928E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="8">
@@ -2159,11 +2207,21 @@
       <c r="C4" s="8">
         <v>3</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="9"/>
+      <c r="D4" s="8">
+        <v>12</v>
+      </c>
+      <c r="E4" s="8">
+        <v>257776423</v>
+      </c>
+      <c r="F4" s="8">
+        <v>100000054</v>
+      </c>
+      <c r="G4" s="8">
+        <v>84012934</v>
+      </c>
+      <c r="H4" s="9">
+        <v>3.8518518518518521E-2</v>
+      </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="8">
@@ -2175,11 +2233,21 @@
       <c r="C5" s="8">
         <v>4</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
+      <c r="D5" s="8">
+        <v>13</v>
+      </c>
+      <c r="E5" s="8">
+        <v>254273656</v>
+      </c>
+      <c r="F5" s="8">
+        <v>100000019</v>
+      </c>
+      <c r="G5" s="8">
+        <v>84013373</v>
+      </c>
+      <c r="H5" s="9">
+        <v>4.3900462962962961E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="8">
@@ -2191,11 +2259,21 @@
       <c r="C6" s="8">
         <v>5</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="9"/>
+      <c r="D6" s="8">
+        <v>13</v>
+      </c>
+      <c r="E6" s="8">
+        <v>260794871</v>
+      </c>
+      <c r="F6" s="8">
+        <v>100000030</v>
+      </c>
+      <c r="G6" s="8">
+        <v>84024338</v>
+      </c>
+      <c r="H6" s="9">
+        <v>4.1585648148148149E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="8">
@@ -2207,11 +2285,21 @@
       <c r="C7" s="8">
         <v>2</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="9"/>
+      <c r="D7" s="8">
+        <v>13</v>
+      </c>
+      <c r="E7" s="8">
+        <v>288926280</v>
+      </c>
+      <c r="F7" s="8">
+        <v>100000034</v>
+      </c>
+      <c r="G7" s="8">
+        <v>84960640</v>
+      </c>
+      <c r="H7" s="9">
+        <v>6.9166666666666668E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="8">
@@ -2223,11 +2311,21 @@
       <c r="C8" s="8">
         <v>3</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="9"/>
+      <c r="D8" s="8">
+        <v>12</v>
+      </c>
+      <c r="E8" s="8">
+        <v>301533163</v>
+      </c>
+      <c r="F8" s="8">
+        <v>100000043</v>
+      </c>
+      <c r="G8" s="8">
+        <v>85385309</v>
+      </c>
+      <c r="H8" s="9">
+        <v>6.7986111111111108E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="8">
@@ -2255,11 +2353,21 @@
       <c r="C10" s="8">
         <v>5</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="12"/>
+      <c r="D10" s="8">
+        <v>11</v>
+      </c>
+      <c r="E10" s="15">
+        <v>298373676</v>
+      </c>
+      <c r="F10" s="15">
+        <v>100000074</v>
+      </c>
+      <c r="G10" s="15">
+        <v>86093036</v>
+      </c>
+      <c r="H10" s="16">
+        <v>8.446759259259258E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="8">
@@ -2287,11 +2395,21 @@
       <c r="C12" s="8">
         <v>3</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="12"/>
+      <c r="D12" s="8">
+        <v>11</v>
+      </c>
+      <c r="E12" s="15">
+        <v>393928418</v>
+      </c>
+      <c r="F12" s="15">
+        <v>100000060</v>
+      </c>
+      <c r="G12" s="15">
+        <v>90506951</v>
+      </c>
+      <c r="H12" s="16">
+        <v>0.45435185185185184</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="8">

</xml_diff>

<commit_message>
Omit the delay between server and client in Durable
</commit_message>
<xml_diff>
--- a/ExperimentRecord.xlsx
+++ b/ExperimentRecord.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dh/Projects/mongodb-tunable-consistency-tla/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EC7D30-3B8B-5D41-8689-83517A909391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068AF0CB-FA8C-5645-A50E-7FCF285AE56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" activeTab="3" xr2:uid="{493B68AF-54D3-6E4F-9EF2-7D5F13399502}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" activeTab="4" xr2:uid="{493B68AF-54D3-6E4F-9EF2-7D5F13399502}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic_problemoverflow" sheetId="1" r:id="rId1"/>
     <sheet name="Basic" sheetId="2" r:id="rId2"/>
     <sheet name="Durable" sheetId="3" r:id="rId3"/>
     <sheet name="Durable2" sheetId="4" r:id="rId4"/>
-    <sheet name="Recoverable" sheetId="5" r:id="rId5"/>
+    <sheet name="PaperData" sheetId="7" r:id="rId5"/>
+    <sheet name="Recoverable" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="21">
   <si>
     <t>TLC模型</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -92,6 +93,18 @@
   </si>
   <si>
     <t>Key Num</t>
+  </si>
+  <si>
+    <t>Basic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Durable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Recoverable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1669,8 +1682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D669FEF8-2D6A-7B4F-B00F-588A1C104E82}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2124,6 +2137,333 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4655F2EE-A5B2-B949-89C4-30770F83A224}">
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="B1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="B2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="8">
+        <v>3</v>
+      </c>
+      <c r="C3" s="8">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8">
+        <v>2</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="6"/>
+      <c r="B4" s="8">
+        <v>3</v>
+      </c>
+      <c r="C4" s="8">
+        <v>2</v>
+      </c>
+      <c r="D4" s="8">
+        <v>3</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="6"/>
+      <c r="B5" s="8">
+        <v>3</v>
+      </c>
+      <c r="C5" s="8">
+        <v>3</v>
+      </c>
+      <c r="D5" s="8">
+        <v>2</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="6"/>
+      <c r="B6" s="8">
+        <v>3</v>
+      </c>
+      <c r="C6" s="8">
+        <v>3</v>
+      </c>
+      <c r="D6" s="8">
+        <v>3</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="8">
+        <v>3</v>
+      </c>
+      <c r="C7" s="8">
+        <v>2</v>
+      </c>
+      <c r="D7" s="8">
+        <v>2</v>
+      </c>
+      <c r="E7" s="8">
+        <v>16</v>
+      </c>
+      <c r="F7" s="8">
+        <v>188250248</v>
+      </c>
+      <c r="G7" s="8">
+        <v>100000046</v>
+      </c>
+      <c r="H7" s="8">
+        <v>69062776</v>
+      </c>
+      <c r="I7" s="9">
+        <v>3.2673611111111105E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="6"/>
+      <c r="B8" s="8">
+        <v>3</v>
+      </c>
+      <c r="C8" s="8">
+        <v>2</v>
+      </c>
+      <c r="D8" s="8">
+        <v>3</v>
+      </c>
+      <c r="E8" s="8">
+        <v>15</v>
+      </c>
+      <c r="F8" s="8">
+        <v>187164763</v>
+      </c>
+      <c r="G8" s="8">
+        <v>100000070</v>
+      </c>
+      <c r="H8" s="8">
+        <v>69500539</v>
+      </c>
+      <c r="I8" s="9">
+        <v>3.3101851851851848E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="6"/>
+      <c r="B9" s="8">
+        <v>3</v>
+      </c>
+      <c r="C9" s="8">
+        <v>3</v>
+      </c>
+      <c r="D9" s="8">
+        <v>2</v>
+      </c>
+      <c r="E9" s="8">
+        <v>13</v>
+      </c>
+      <c r="F9" s="8">
+        <v>200055783</v>
+      </c>
+      <c r="G9" s="8">
+        <v>100000020</v>
+      </c>
+      <c r="H9" s="8">
+        <v>67966847</v>
+      </c>
+      <c r="I9" s="9">
+        <v>4.4247685185185182E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="6"/>
+      <c r="B10" s="8">
+        <v>3</v>
+      </c>
+      <c r="C10" s="8">
+        <v>3</v>
+      </c>
+      <c r="D10" s="8">
+        <v>3</v>
+      </c>
+      <c r="E10" s="8">
+        <v>12</v>
+      </c>
+      <c r="F10" s="8">
+        <v>194223872</v>
+      </c>
+      <c r="G10" s="8">
+        <v>100000046</v>
+      </c>
+      <c r="H10" s="8">
+        <v>71372004</v>
+      </c>
+      <c r="I10" s="9">
+        <v>4.5543981481481477E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="8">
+        <v>3</v>
+      </c>
+      <c r="C11" s="8">
+        <v>2</v>
+      </c>
+      <c r="D11" s="8">
+        <v>2</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="6"/>
+      <c r="B12" s="8">
+        <v>3</v>
+      </c>
+      <c r="C12" s="8">
+        <v>2</v>
+      </c>
+      <c r="D12" s="8">
+        <v>3</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="6"/>
+      <c r="B13" s="8">
+        <v>3</v>
+      </c>
+      <c r="C13" s="8">
+        <v>3</v>
+      </c>
+      <c r="D13" s="8">
+        <v>2</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="6"/>
+      <c r="B14" s="8">
+        <v>3</v>
+      </c>
+      <c r="C14" s="8">
+        <v>3</v>
+      </c>
+      <c r="D14" s="8">
+        <v>3</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B6E2F82-D946-0145-A470-82D88D964591}">
   <dimension ref="A1:H18"/>
   <sheetViews>

</xml_diff>